<commit_message>
tabel ms excel upload
</commit_message>
<xml_diff>
--- a/table.xlsx
+++ b/table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\work\git\data-structure\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D6115511-EF72-4DD3-8B33-4D01993BAFC5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1ED86FF-B0EF-4926-B31D-E44701408F57}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -469,408 +468,408 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:M24"/>
+  <dimension ref="C2:N24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="33.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="24.08984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.90625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.453125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="33.54296875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="27.08984375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.1796875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="24.08984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.90625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="33.54296875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="27.08984375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B2" t="s">
+    <row r="2" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="C2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
-        <v>1</v>
-      </c>
       <c r="D2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>3</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>4</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>5</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>6</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>7</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>8</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>9</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>10</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="C4" t="s">
+    <row r="4" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="D4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="C5" t="s">
+    <row r="5" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="D5" t="s">
         <v>12</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="C6" t="s">
+    <row r="6" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="D6" t="s">
         <v>12</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>13</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="C7" t="s">
+    <row r="7" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="D7" t="s">
         <v>12</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>13</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>14</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="G8" t="s">
+    <row r="8" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="H8" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="H9" t="s">
+    <row r="9" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="I9" t="s">
         <v>17</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>0</v>
       </c>
-      <c r="J9" t="s">
+      <c r="K9" t="s">
         <v>12</v>
       </c>
-      <c r="K9" t="s">
+      <c r="L9" t="s">
         <v>28</v>
       </c>
-      <c r="L9">
+      <c r="M9">
         <v>0</v>
       </c>
-      <c r="M9" t="s">
+      <c r="N9" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="J10" t="s">
+    <row r="10" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="K10" t="s">
         <v>12</v>
       </c>
-      <c r="K10" t="s">
+      <c r="L10" t="s">
         <v>20</v>
       </c>
-      <c r="L10">
-        <v>1</v>
-      </c>
-      <c r="M10" t="s">
+      <c r="M10">
+        <v>1</v>
+      </c>
+      <c r="N10" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="J11" t="s">
+    <row r="11" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="K11" t="s">
         <v>12</v>
       </c>
-      <c r="K11" t="s">
+      <c r="L11" t="s">
         <v>22</v>
       </c>
-      <c r="L11">
+      <c r="M11">
         <v>2</v>
       </c>
-      <c r="M11" t="s">
+      <c r="N11" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="J12" t="s">
+    <row r="12" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="K12" t="s">
         <v>12</v>
       </c>
-      <c r="K12" t="s">
+      <c r="L12" t="s">
         <v>24</v>
       </c>
-      <c r="L12">
+      <c r="M12">
         <v>3</v>
       </c>
-      <c r="M12" t="s">
+      <c r="N12" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="H13" t="s">
-        <v>25</v>
-      </c>
-      <c r="I13">
-        <v>1</v>
-      </c>
-      <c r="J13" t="s">
+    <row r="13" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="I13" t="s">
+        <v>25</v>
+      </c>
+      <c r="J13">
+        <v>1</v>
+      </c>
+      <c r="K13" t="s">
         <v>13</v>
       </c>
-      <c r="K13" t="s">
+      <c r="L13" t="s">
         <v>27</v>
       </c>
-      <c r="L13">
+      <c r="M13">
         <v>0</v>
       </c>
-      <c r="M13" t="s">
+      <c r="N13" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="H14" t="s">
-        <v>25</v>
-      </c>
-      <c r="I14">
-        <v>1</v>
-      </c>
-      <c r="J14" t="s">
+    <row r="14" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="I14" t="s">
+        <v>25</v>
+      </c>
+      <c r="J14">
+        <v>1</v>
+      </c>
+      <c r="K14" t="s">
         <v>13</v>
       </c>
-      <c r="K14" t="s">
+      <c r="L14" t="s">
         <v>29</v>
       </c>
-      <c r="L14">
-        <v>1</v>
-      </c>
       <c r="M14">
+        <v>1</v>
+      </c>
+      <c r="N14">
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="H15" t="s">
-        <v>25</v>
-      </c>
-      <c r="I15">
-        <v>1</v>
-      </c>
-      <c r="J15" t="s">
+    <row r="15" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="I15" t="s">
+        <v>25</v>
+      </c>
+      <c r="J15">
+        <v>1</v>
+      </c>
+      <c r="K15" t="s">
         <v>13</v>
       </c>
-      <c r="K15" t="s">
+      <c r="L15" t="s">
         <v>30</v>
       </c>
-      <c r="L15">
+      <c r="M15">
         <v>2</v>
       </c>
-      <c r="M15">
+      <c r="N15">
         <v>55</v>
       </c>
     </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="H16" t="s">
-        <v>25</v>
-      </c>
-      <c r="I16">
-        <v>1</v>
-      </c>
-      <c r="J16" t="s">
+    <row r="16" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="I16" t="s">
+        <v>25</v>
+      </c>
+      <c r="J16">
+        <v>1</v>
+      </c>
+      <c r="K16" t="s">
         <v>13</v>
       </c>
-      <c r="K16" t="s">
+      <c r="L16" t="s">
         <v>31</v>
       </c>
-      <c r="L16">
+      <c r="M16">
         <v>3</v>
       </c>
-      <c r="M16">
+      <c r="N16">
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="8:13" x14ac:dyDescent="0.35">
-      <c r="H17" t="s">
-        <v>25</v>
-      </c>
-      <c r="I17">
+    <row r="17" spans="9:14" x14ac:dyDescent="0.35">
+      <c r="I17" t="s">
+        <v>25</v>
+      </c>
+      <c r="J17">
         <v>2</v>
       </c>
-      <c r="J17" t="s">
+      <c r="K17" t="s">
         <v>14</v>
       </c>
-      <c r="K17" t="s">
+      <c r="L17" t="s">
         <v>33</v>
       </c>
-      <c r="L17">
+      <c r="M17">
         <v>0</v>
       </c>
-      <c r="M17" t="s">
+      <c r="N17" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="8:13" x14ac:dyDescent="0.35">
-      <c r="H18" t="s">
-        <v>25</v>
-      </c>
-      <c r="I18">
+    <row r="18" spans="9:14" x14ac:dyDescent="0.35">
+      <c r="I18" t="s">
+        <v>25</v>
+      </c>
+      <c r="J18">
         <v>2</v>
       </c>
-      <c r="J18" t="s">
+      <c r="K18" t="s">
         <v>14</v>
       </c>
-      <c r="K18" t="s">
+      <c r="L18" t="s">
         <v>34</v>
       </c>
-      <c r="L18">
-        <v>1</v>
-      </c>
       <c r="M18">
+        <v>1</v>
+      </c>
+      <c r="N18">
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="8:13" x14ac:dyDescent="0.35">
-      <c r="H19" t="s">
-        <v>25</v>
-      </c>
-      <c r="I19">
+    <row r="19" spans="9:14" x14ac:dyDescent="0.35">
+      <c r="I19" t="s">
+        <v>25</v>
+      </c>
+      <c r="J19">
         <v>2</v>
       </c>
-      <c r="J19" t="s">
+      <c r="K19" t="s">
         <v>14</v>
       </c>
-      <c r="K19" t="s">
+      <c r="L19" t="s">
         <v>35</v>
       </c>
-      <c r="L19">
+      <c r="M19">
         <v>2</v>
       </c>
-      <c r="M19">
+      <c r="N19">
         <v>66</v>
       </c>
     </row>
-    <row r="20" spans="8:13" x14ac:dyDescent="0.35">
-      <c r="H20" t="s">
-        <v>25</v>
-      </c>
-      <c r="I20">
+    <row r="20" spans="9:14" x14ac:dyDescent="0.35">
+      <c r="I20" t="s">
+        <v>25</v>
+      </c>
+      <c r="J20">
         <v>2</v>
       </c>
-      <c r="J20" t="s">
+      <c r="K20" t="s">
         <v>14</v>
       </c>
-      <c r="K20" t="s">
+      <c r="L20" t="s">
         <v>36</v>
       </c>
-      <c r="L20">
+      <c r="M20">
         <v>3</v>
       </c>
-      <c r="M20">
+      <c r="N20">
         <v>67</v>
       </c>
     </row>
-    <row r="21" spans="8:13" x14ac:dyDescent="0.35">
-      <c r="H21" t="s">
-        <v>25</v>
-      </c>
-      <c r="I21">
+    <row r="21" spans="9:14" x14ac:dyDescent="0.35">
+      <c r="I21" t="s">
+        <v>25</v>
+      </c>
+      <c r="J21">
         <v>3</v>
       </c>
-      <c r="J21" t="s">
+      <c r="K21" t="s">
         <v>15</v>
       </c>
-      <c r="K21" t="s">
+      <c r="L21" t="s">
         <v>38</v>
       </c>
-      <c r="L21">
+      <c r="M21">
         <v>0</v>
       </c>
-      <c r="M21" t="s">
+      <c r="N21" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="8:13" x14ac:dyDescent="0.35">
-      <c r="H22" t="s">
-        <v>25</v>
-      </c>
-      <c r="I22">
+    <row r="22" spans="9:14" x14ac:dyDescent="0.35">
+      <c r="I22" t="s">
+        <v>25</v>
+      </c>
+      <c r="J22">
         <v>3</v>
       </c>
-      <c r="J22" t="s">
+      <c r="K22" t="s">
         <v>15</v>
       </c>
-      <c r="K22" t="s">
+      <c r="L22" t="s">
         <v>39</v>
       </c>
-      <c r="L22">
-        <v>1</v>
-      </c>
       <c r="M22">
+        <v>1</v>
+      </c>
+      <c r="N22">
         <v>60</v>
       </c>
     </row>
-    <row r="23" spans="8:13" x14ac:dyDescent="0.35">
-      <c r="H23" t="s">
-        <v>25</v>
-      </c>
-      <c r="I23">
+    <row r="23" spans="9:14" x14ac:dyDescent="0.35">
+      <c r="I23" t="s">
+        <v>25</v>
+      </c>
+      <c r="J23">
         <v>3</v>
       </c>
-      <c r="J23" t="s">
+      <c r="K23" t="s">
         <v>15</v>
       </c>
-      <c r="K23" t="s">
+      <c r="L23" t="s">
         <v>40</v>
       </c>
-      <c r="L23">
+      <c r="M23">
         <v>2</v>
       </c>
-      <c r="M23">
+      <c r="N23">
         <v>65</v>
       </c>
     </row>
-    <row r="24" spans="8:13" x14ac:dyDescent="0.35">
-      <c r="H24" t="s">
-        <v>25</v>
-      </c>
-      <c r="I24">
+    <row r="24" spans="9:14" x14ac:dyDescent="0.35">
+      <c r="I24" t="s">
+        <v>25</v>
+      </c>
+      <c r="J24">
         <v>3</v>
       </c>
-      <c r="J24" t="s">
+      <c r="K24" t="s">
         <v>15</v>
       </c>
-      <c r="K24" t="s">
+      <c r="L24" t="s">
         <v>41</v>
       </c>
-      <c r="L24">
+      <c r="M24">
         <v>3</v>
       </c>
-      <c r="M24">
+      <c r="N24">
         <v>69</v>
       </c>
     </row>

</xml_diff>